<commit_message>
Anwenderdokumentation & Projektbericht aktualisiert
</commit_message>
<xml_diff>
--- a/Dokumente/Projektbericht.xlsx
+++ b/Dokumente/Projektbericht.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Dokumente\Software Engineering\Beleg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Temp\suluSearch\Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF6000B-7D85-49BA-A0AC-03AC148D2AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>SULUsearch Projektbericht</t>
   </si>
@@ -168,12 +169,36 @@
   </si>
   <si>
     <t>2 Stunden</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>1.5 Stunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --- </t>
+  </si>
+  <si>
+    <t>0.25 Stunden</t>
+  </si>
+  <si>
+    <t>0.5 Stunden</t>
+  </si>
+  <si>
+    <t>Update und Dokument-Aktualisierungen</t>
+  </si>
+  <si>
+    <t>2.5 Stunden</t>
+  </si>
+  <si>
+    <t>8 Stunden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -266,6 +291,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,11 +574,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +738,9 @@
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D14" s="9">
         <v>43545</v>
       </c>
@@ -725,7 +755,9 @@
       <c r="B15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="9">
         <v>43552</v>
       </c>
@@ -740,7 +772,9 @@
       <c r="B16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D16" s="9">
         <v>43559</v>
       </c>
@@ -755,7 +789,9 @@
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D17" s="9">
         <v>43580</v>
       </c>
@@ -770,7 +806,9 @@
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="D18" s="9">
         <v>43591</v>
       </c>
@@ -785,7 +823,9 @@
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D19" s="9">
         <v>43595</v>
       </c>
@@ -797,8 +837,12 @@
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="D20" s="9">
         <v>43600</v>
       </c>
@@ -813,11 +857,31 @@
       <c r="B21" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D21" s="9">
-        <v>43646</v>
+        <v>43609</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="14">
+        <v>43637</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>